<commit_message>
Add subscription management tests
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07069D5D-4BF9-4036-9337-3729F38053F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A418DC2-7AC4-4A60-B4A4-C096FF0D719A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="22656" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerSubscriptions" sheetId="8" r:id="rId1"/>
-    <sheet name="getSubscriptions" sheetId="9" r:id="rId2"/>
-    <sheet name="delSubscriptionById" sheetId="10" r:id="rId3"/>
+    <sheet name="delSubscriptionById" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>description</t>
   </si>
@@ -47,18 +46,12 @@
     <t>Successfully</t>
   </si>
   <si>
-    <t>bad request</t>
-  </si>
-  <si>
     <t>clientId</t>
   </si>
   <si>
     <t>subSentence</t>
   </si>
   <si>
-    <t>iems</t>
-  </si>
-  <si>
     <t>subscription {SensorData(cond:"{Siid:{_in:[34131]}}") {Siid updateTime value}}</t>
   </si>
   <si>
@@ -80,21 +73,9 @@
     <t>iEMS-sub-mgmt-Test-4-var4</t>
   </si>
   <si>
-    <t>iems2</t>
-  </si>
-  <si>
     <t>iEMS-sub-mgmt-Test-4-var5</t>
   </si>
   <si>
-    <t>iems~!@#$%^&amp;*()_+-={}[]|\"'::&lt;&gt;.??</t>
-  </si>
-  <si>
-    <t>iems,iems2</t>
-  </si>
-  <si>
-    <t>iems,iems2,iems~!@#$%^&amp;*()_+-={}[]|\"'::&lt;&gt;.??</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -140,9 +121,6 @@
     <t>Subscription not_exist not exists!</t>
   </si>
   <si>
-    <t>iems_incorrect</t>
-  </si>
-  <si>
     <t>iEMS-sub-mgmt-Tes-3-var3</t>
   </si>
   <si>
@@ -161,68 +139,70 @@
     <t>subscription {SensorData (cond:"{Siid:{_in:[34131]}}") {Siid_error updateTime value}}</t>
   </si>
   <si>
-    <t>fields</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-1-var1</t>
-  </si>
-  <si>
-    <t>GetSubMgmt</t>
-  </si>
-  <si>
-    <t>id,entities,clients</t>
-  </si>
-  <si>
     <t>good request</t>
   </si>
   <si>
-    <t>good request, repeat register subscription</t>
-  </si>
-  <si>
-    <t>good request, clinetId coitain special characters</t>
-  </si>
-  <si>
-    <t>good request, different clinetId</t>
-  </si>
-  <si>
-    <t>subscription {Analog(cond:"{Siid:{_in:[35906,33329]}}")
-{localName mRID maxValue measurementType minValue name normalValue pathName positiveFlowIn generate_SensorData(cond:""){Siid modelId partition updateTime value}}}</t>
-  </si>
-  <si>
-    <t>bad request, an extra quotes</t>
-  </si>
-  <si>
-    <t>bad request, wrong entity</t>
-  </si>
-  <si>
-    <t>bad request,An inverted brace is missing</t>
-  </si>
-  <si>
-    <t>bad request, wrong field</t>
-  </si>
-  <si>
-    <t>bad request, both clientid and id were blank space</t>
-  </si>
-  <si>
     <t>bad request, id not exist</t>
   </si>
   <si>
-    <t>good request, correct both clientId and id</t>
-  </si>
-  <si>
-    <t>bad request, id exist but clientId not exist</t>
-  </si>
-  <si>
     <t>not exist</t>
   </si>
   <si>
     <t>iEMS-sub-mgmt-Tes-3-var5</t>
   </si>
   <si>
-    <t>bad request, Repeat delete subscription</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> not exists</t>
+    <t>testClient01</t>
+  </si>
+  <si>
+    <t>testClient02</t>
+  </si>
+  <si>
+    <t>testClient01~!@#$%^&amp;*()_+-={}[]|\"'::&lt;&gt;.??</t>
+  </si>
+  <si>
+    <t>testClient01_incorrect</t>
+  </si>
+  <si>
+    <t>good request, repeat the same subscription</t>
+  </si>
+  <si>
+    <t>good request, submit same subscription with different clientId</t>
+  </si>
+  <si>
+    <t>good request, clientId contains special characters</t>
+  </si>
+  <si>
+    <t>subscription { SensorData (cond: "{Siid:{_in:[34155,34159,34155]}}") {Siid updateTime value } }</t>
+  </si>
+  <si>
+    <t>good request, single device subscription</t>
+  </si>
+  <si>
+    <t>good request, multipe devices subscription</t>
+  </si>
+  <si>
+    <t>bad request, improper quotes</t>
+  </si>
+  <si>
+    <t>bad request, incorrect entity name</t>
+  </si>
+  <si>
+    <t>bad request, missing an inverted brace</t>
+  </si>
+  <si>
+    <t>bad request, incorrect field</t>
+  </si>
+  <si>
+    <t>not exists</t>
+  </si>
+  <si>
+    <t>bad request, valid id with invalid clientId</t>
+  </si>
+  <si>
+    <t>bad request, delete the same subscription twice</t>
+  </si>
+  <si>
+    <t>bad request, both clientid and id are empty</t>
   </si>
 </sst>
 </file>
@@ -303,8 +283,12 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -314,15 +298,27 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,21 +601,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C42AED7-09F1-48C2-896C-1C950898C255}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" customWidth="1"/>
-    <col min="2" max="2" width="81.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="69.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="48.6328125" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -627,13 +623,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -644,166 +640,169 @@
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="4">
+        <v>200</v>
+      </c>
+      <c r="G2" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4">
+        <v>200</v>
+      </c>
+      <c r="G3" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="4">
+        <v>200</v>
+      </c>
+      <c r="G4" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="4">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="2">
-        <v>200</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="E6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4">
+        <v>200</v>
+      </c>
+      <c r="G6" s="4">
         <v>100000</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="2">
-        <v>200</v>
-      </c>
-      <c r="G3" s="2">
-        <v>100000</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="I6" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2">
-        <v>200</v>
-      </c>
-      <c r="G4" s="2">
-        <v>100000</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2">
-        <v>200</v>
-      </c>
-      <c r="G5" s="2">
-        <v>100000</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="178.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2">
-        <v>200</v>
-      </c>
-      <c r="G6" s="2">
-        <v>107001</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="E7" s="7"/>
       <c r="F7" s="5">
         <v>200</v>
       </c>
@@ -811,25 +810,26 @@
         <v>107001</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E8" s="7"/>
       <c r="F8" s="5">
         <v>200</v>
       </c>
@@ -837,25 +837,26 @@
         <v>107001</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="5">
         <v>200</v>
       </c>
@@ -863,25 +864,26 @@
         <v>107001</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="5">
         <v>200</v>
       </c>
@@ -889,94 +891,40 @@
         <v>107001</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0DDC05-CA4C-40D3-8FC6-91491D583EA7}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="5">
-        <v>200</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C864B5-904B-4803-87FD-A0148A25AFB7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="48.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="6" width="25.21875" customWidth="1"/>
-    <col min="9" max="9" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="25.1796875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.7265625" style="3"/>
+    <col min="9" max="9" width="29.36328125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -984,16 +932,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1004,25 +952,25 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="6"/>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="5"/>
       <c r="G2" s="5">
         <v>200</v>
       </c>
@@ -1030,27 +978,27 @@
         <v>107002</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="6"/>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="5">
         <v>200</v>
       </c>
@@ -1058,26 +1006,25 @@
         <v>107002</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5">
         <v>200</v>
       </c>
@@ -1085,25 +1032,26 @@
         <v>107002</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>41</v>
+        <v>41</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="G5" s="5">
         <v>200</v>
@@ -1114,21 +1062,21 @@
       <c r="I5" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="5">
         <v>200</v>
       </c>
@@ -1136,15 +1084,15 @@
         <v>107002</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
+        <v>55</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change submgmt test data, status code 400->200
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C886E7-6EE0-4E5C-9538-A798AD4CF64A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4956F4B6-294E-4DCD-9F8A-7488CEC8032F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerSubscriptions" sheetId="8" r:id="rId1"/>
@@ -601,21 +601,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C42AED7-09F1-48C2-896C-1C950898C255}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="69.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="48.6328125" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,7 +644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -673,7 +673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -702,7 +702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
@@ -731,7 +731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
@@ -760,7 +760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -789,7 +789,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -803,8 +803,8 @@
         <v>13</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="5">
-        <v>400</v>
+      <c r="F7" s="4">
+        <v>200</v>
       </c>
       <c r="G7" s="5">
         <v>107001</v>
@@ -816,7 +816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -830,8 +830,8 @@
         <v>14</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="5">
-        <v>400</v>
+      <c r="F8" s="4">
+        <v>200</v>
       </c>
       <c r="G8" s="5">
         <v>107001</v>
@@ -843,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -857,8 +857,8 @@
         <v>15</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="5">
-        <v>400</v>
+      <c r="F9" s="4">
+        <v>200</v>
       </c>
       <c r="G9" s="5">
         <v>107001</v>
@@ -870,7 +870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -884,8 +884,8 @@
         <v>23</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="5">
-        <v>400</v>
+      <c r="F10" s="4">
+        <v>200</v>
       </c>
       <c r="G10" s="5">
         <v>107001</v>
@@ -908,23 +908,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C864B5-904B-4803-87FD-A0148A25AFB7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="25.21875" style="3" customWidth="1"/>
-    <col min="7" max="8" width="8.77734375" style="3"/>
-    <col min="9" max="9" width="29.33203125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="25.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="25.1796875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.81640625" style="3"/>
+    <col min="9" max="9" width="29.36328125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -956,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>54</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H2" s="5">
         <v>107002</v>
@@ -984,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H3" s="5">
         <v>107002</v>
@@ -1012,7 +1012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>56</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>58</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H6" s="5">
         <v>107002</v>

</xml_diff>

<commit_message>
change test data for iems-submgmt-test-14, error code 107002->107003
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4956F4B6-294E-4DCD-9F8A-7488CEC8032F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94298FEF-433D-4FAF-9FDA-EF04EDE45DD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerSubscriptions" sheetId="8" r:id="rId1"/>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C42AED7-09F1-48C2-896C-1C950898C255}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C864B5-904B-4803-87FD-A0148A25AFB7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1081,7 +1081,7 @@
         <v>200</v>
       </c>
       <c r="H6" s="5">
-        <v>107002</v>
+        <v>107003</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
update for DelSubMgmt missing name
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94298FEF-433D-4FAF-9FDA-EF04EDE45DD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8AA835-FE0F-43C8-A325-A91FF745857C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1836" yWindow="1728" windowWidth="19740" windowHeight="12072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerSubscriptions" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>description</t>
   </si>
@@ -94,115 +94,116 @@
     <t>RegisterSubMgmt</t>
   </si>
   <si>
+    <t>subscription {SensorData (cond:"{Siid:{_in:[34131]}}") {Siid_error updateTime value}}</t>
+  </si>
+  <si>
+    <t>good request</t>
+  </si>
+  <si>
+    <t>bad request, id not exist</t>
+  </si>
+  <si>
+    <t>not exist</t>
+  </si>
+  <si>
+    <t>testClient01</t>
+  </si>
+  <si>
+    <t>testClient02</t>
+  </si>
+  <si>
+    <t>testClient01~!@#$%^&amp;*()_+-={}[]|\"'::&lt;&gt;.??</t>
+  </si>
+  <si>
+    <t>testClient01_incorrect</t>
+  </si>
+  <si>
+    <t>good request, repeat the same subscription</t>
+  </si>
+  <si>
+    <t>good request, submit same subscription with different clientId</t>
+  </si>
+  <si>
+    <t>good request, clientId contains special characters</t>
+  </si>
+  <si>
+    <t>subscription { SensorData (cond: "{Siid:{_in:[34155,34159,34155]}}") {Siid updateTime value } }</t>
+  </si>
+  <si>
+    <t>good request, single device subscription</t>
+  </si>
+  <si>
+    <t>good request, multipe devices subscription</t>
+  </si>
+  <si>
+    <t>bad request, improper quotes</t>
+  </si>
+  <si>
+    <t>bad request, incorrect entity name</t>
+  </si>
+  <si>
+    <t>bad request, missing an inverted brace</t>
+  </si>
+  <si>
+    <t>bad request, incorrect field</t>
+  </si>
+  <si>
+    <t>not exists</t>
+  </si>
+  <si>
+    <t>bad request, valid id with invalid clientId</t>
+  </si>
+  <si>
+    <t>bad request, delete the same subscription twice</t>
+  </si>
+  <si>
+    <t>bad request, both clientid and id are empty</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-1</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-2</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-3</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-4</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-5</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-6</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-7</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-8</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Test-9</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Tes-10</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Tes-11</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Tes-12</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Tes-13</t>
+  </si>
+  <si>
+    <t>iEMS-sub-mgmt-Tes-14</t>
+  </si>
+  <si>
     <t>DelSubMgmt</t>
-  </si>
-  <si>
-    <t>subscription {SensorData (cond:"{Siid:{_in:[34131]}}") {Siid_error updateTime value}}</t>
-  </si>
-  <si>
-    <t>good request</t>
-  </si>
-  <si>
-    <t>bad request, id not exist</t>
-  </si>
-  <si>
-    <t>not exist</t>
-  </si>
-  <si>
-    <t>testClient01</t>
-  </si>
-  <si>
-    <t>testClient02</t>
-  </si>
-  <si>
-    <t>testClient01~!@#$%^&amp;*()_+-={}[]|\"'::&lt;&gt;.??</t>
-  </si>
-  <si>
-    <t>testClient01_incorrect</t>
-  </si>
-  <si>
-    <t>good request, repeat the same subscription</t>
-  </si>
-  <si>
-    <t>good request, submit same subscription with different clientId</t>
-  </si>
-  <si>
-    <t>good request, clientId contains special characters</t>
-  </si>
-  <si>
-    <t>subscription { SensorData (cond: "{Siid:{_in:[34155,34159,34155]}}") {Siid updateTime value } }</t>
-  </si>
-  <si>
-    <t>good request, single device subscription</t>
-  </si>
-  <si>
-    <t>good request, multipe devices subscription</t>
-  </si>
-  <si>
-    <t>bad request, improper quotes</t>
-  </si>
-  <si>
-    <t>bad request, incorrect entity name</t>
-  </si>
-  <si>
-    <t>bad request, missing an inverted brace</t>
-  </si>
-  <si>
-    <t>bad request, incorrect field</t>
-  </si>
-  <si>
-    <t>not exists</t>
-  </si>
-  <si>
-    <t>bad request, valid id with invalid clientId</t>
-  </si>
-  <si>
-    <t>bad request, delete the same subscription twice</t>
-  </si>
-  <si>
-    <t>bad request, both clientid and id are empty</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-1</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-2</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-3</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-4</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-5</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-6</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-7</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-8</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Test-9</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Tes-10</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Tes-11</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Tes-12</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Tes-13</t>
-  </si>
-  <si>
-    <t>iEMS-sub-mgmt-Tes-14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -213,20 +214,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -605,17 +606,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" customWidth="1"/>
-    <col min="2" max="2" width="48.6328125" customWidth="1"/>
-    <col min="3" max="3" width="36.6328125" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
-    <col min="9" max="9" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="69.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,15 +645,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -670,18 +671,18 @@
         <v>5</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -699,18 +700,18 @@
         <v>5</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
@@ -728,18 +729,18 @@
         <v>5</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -757,21 +758,21 @@
         <v>5</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>21</v>
@@ -786,18 +787,18 @@
         <v>5</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>13</v>
@@ -816,15 +817,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>14</v>
@@ -843,15 +844,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>15</v>
@@ -870,18 +871,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="4">
@@ -908,23 +909,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C864B5-904B-4803-87FD-A0148A25AFB7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="25.1796875" style="3" customWidth="1"/>
-    <col min="7" max="8" width="8.81640625" style="3"/>
-    <col min="9" max="9" width="29.36328125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="25.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="25.21875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.77734375" style="3"/>
+    <col min="9" max="9" width="29.33203125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -956,12 +957,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>18</v>
@@ -984,15 +985,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
@@ -1012,15 +1013,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="5"/>
@@ -1032,26 +1033,26 @@
         <v>107002</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="G5" s="5">
         <v>200</v>
@@ -1064,19 +1065,21 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="G6" s="5">
         <v>200</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>107003</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
add new schema template file
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8AA835-FE0F-43C8-A325-A91FF745857C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C3E749-FDB6-49D4-850C-2F8DC1054CE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1836" yWindow="1728" windowWidth="19740" windowHeight="12072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerSubscriptions" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>description</t>
   </si>
@@ -203,6 +203,14 @@
   </si>
   <si>
     <t>DelSubMgmt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DelSubMgmtNull</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -603,7 +611,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -909,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C864B5-904B-4803-87FD-A0148A25AFB7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -969,7 +977,7 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5">
@@ -1078,7 +1086,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G6" s="5">
         <v>200</v>

</xml_diff>

<commit_message>
fix iEMS-sub-mgmt-Test-12, test is not executed at all
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C3E749-FDB6-49D4-850C-2F8DC1054CE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88869BE2-BF90-4422-BC00-1FA6B1816E03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerSubscriptions" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>description</t>
   </si>
@@ -103,9 +103,6 @@
     <t>bad request, id not exist</t>
   </si>
   <si>
-    <t>not exist</t>
-  </si>
-  <si>
     <t>testClient01</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t>testClient01~!@#$%^&amp;*()_+-={}[]|\"'::&lt;&gt;.??</t>
-  </si>
-  <si>
-    <t>testClient01_incorrect</t>
   </si>
   <si>
     <t>good request, repeat the same subscription</t>
@@ -222,20 +216,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -614,17 +608,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="69.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="2" max="2" width="48.6328125" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -653,15 +647,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -679,18 +673,18 @@
         <v>5</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -708,18 +702,18 @@
         <v>5</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
@@ -737,18 +731,18 @@
         <v>5</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -766,21 +760,21 @@
         <v>5</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>21</v>
@@ -795,18 +789,18 @@
         <v>5</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>13</v>
@@ -825,15 +819,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>14</v>
@@ -852,15 +846,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>15</v>
@@ -879,15 +873,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>22</v>
@@ -918,22 +912,22 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="25.21875" style="3" customWidth="1"/>
-    <col min="7" max="8" width="8.77734375" style="3"/>
-    <col min="9" max="9" width="29.33203125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="25.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="25.1796875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.81640625" style="3"/>
+    <col min="9" max="9" width="29.36328125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -965,19 +959,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5">
@@ -993,15 +987,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
@@ -1021,46 +1015,46 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H4" s="5">
-        <v>107002</v>
+        <v>107003</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G5" s="5">
         <v>200</v>
@@ -1073,20 +1067,20 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G6" s="5">
         <v>200</v>
@@ -1095,7 +1089,7 @@
         <v>107003</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
modify iems-subscription-management-test-data.xlsx for the response code 'iEMS-sub-mgmt-Test-4'
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-subscription-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C251197C-7CC7-410E-974D-2BE88E69970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C97722-A4E4-4FCF-9610-86943EE36318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerSubscriptions" sheetId="8" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C42AED7-09F1-48C2-896C-1C950898C255}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -620,8 +620,8 @@
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -762,11 +762,11 @@
       <c r="G5" s="4">
         <v>101400</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>59</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C864B5-904B-4803-87FD-A0148A25AFB7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>